<commit_message>
Importar Datos Fast Excel y otro
</commit_message>
<xml_diff>
--- a/public/DataUpload/users-encabezados-1.xlsx
+++ b/public/DataUpload/users-encabezados-1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="26">
   <si>
     <t xml:space="preserve">first_name</t>
   </si>
@@ -79,10 +79,16 @@
     <t xml:space="preserve">Dr. Wilford Rempel</t>
   </si>
   <si>
+    <t xml:space="preserve">Rempel</t>
+  </si>
+  <si>
     <t xml:space="preserve">amedhurst@example.net</t>
   </si>
   <si>
     <t xml:space="preserve">Ms. Damaris Luettgen MD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Damaris Luettgen MD</t>
   </si>
   <si>
     <t xml:space="preserve">randi.breitenberg@example.org</t>
@@ -191,10 +197,10 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="27.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="30.47"/>
@@ -318,10 +324,10 @@
         <v>18</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D9" s="0" t="s">
         <v>3</v>
@@ -329,13 +335,13 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D10" s="0" t="s">
         <v>3</v>
@@ -343,13 +349,13 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D11" s="0" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
Importar Datos Relacionados con Fast Excel y otro
</commit_message>
<xml_diff>
--- a/public/DataUpload/users-encabezados-1.xlsx
+++ b/public/DataUpload/users-encabezados-1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="30">
   <si>
     <t xml:space="preserve">first_name</t>
   </si>
@@ -34,22 +34,34 @@
     <t xml:space="preserve">password</t>
   </si>
   <si>
+    <t xml:space="preserve">acronym</t>
+  </si>
+  <si>
     <t xml:space="preserve">Marielle Predovic</t>
   </si>
   <si>
     <t xml:space="preserve">roy.krajcik@example.net</t>
   </si>
   <si>
+    <t xml:space="preserve">area_a</t>
+  </si>
+  <si>
     <t xml:space="preserve">Vada Weber</t>
   </si>
   <si>
     <t xml:space="preserve">herman40@example.com</t>
   </si>
   <si>
+    <t xml:space="preserve">area_b</t>
+  </si>
+  <si>
     <t xml:space="preserve">Pascale Maggio</t>
   </si>
   <si>
     <t xml:space="preserve">isabel73@example.org</t>
+  </si>
+  <si>
+    <t xml:space="preserve">area_c</t>
   </si>
   <si>
     <t xml:space="preserve">Prof. Santiago Bartoletti</t>
@@ -172,9 +184,13 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -194,13 +210,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="27.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="30.47"/>
@@ -220,145 +236,178 @@
       <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>3</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>3</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>3</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>3</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>3</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D7" s="0" t="s">
         <v>3</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D8" s="0" t="s">
         <v>3</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D9" s="0" t="s">
         <v>3</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D10" s="0" t="s">
         <v>3</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="D11" s="0" t="s">
         <v>3</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>